<commit_message>
Major Changes (MetaData, CRUD, TotalBooksInfo)
</commit_message>
<xml_diff>
--- a/ERDiagram-TableSchema/AS2_Excel.xlsx
+++ b/ERDiagram-TableSchema/AS2_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADA\Subjects\Database Systems\AS2\PSQL\Schema-Diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADA\Subjects\Database Systems\AS2_Git_DBS\ERDiagram-TableSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF560FC6-A5BE-4D04-AB45-5133515C5073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4EBBEF-D554-4A35-A81C-4A464381EB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -235,11 +235,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -252,17 +283,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:P19"/>
+  <dimension ref="A2:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,148 +605,120 @@
     <col min="9" max="9" width="12.77734375" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" customWidth="1"/>
     <col min="16" max="16" width="13.88671875" customWidth="1"/>
     <col min="17" max="17" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="13"/>
+      <c r="J2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="16"/>
-      <c r="O2" s="14" t="s">
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="16"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O2" s="13"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
       <c r="H4" s="4"/>
       <c r="J4" s="5"/>
-      <c r="M4" s="4"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K4" s="16"/>
+      <c r="L4" s="4"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
       <c r="H5" s="4"/>
       <c r="J5" s="5"/>
-      <c r="M5" s="4"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K5" s="16"/>
+      <c r="L5" s="4"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
       <c r="H6" s="4"/>
       <c r="J6" s="5"/>
-      <c r="M6" s="4"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K6" s="16"/>
+      <c r="L6" s="4"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
       <c r="H7" s="4"/>
       <c r="J7" s="5"/>
-      <c r="M7" s="4"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K7" s="16"/>
+      <c r="L7" s="4"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
       <c r="H8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="M8" s="4"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K8" s="16"/>
+      <c r="L8" s="4"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -712,32 +729,35 @@
       <c r="H9" s="8"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C12" s="14" t="s">
+      <c r="L9" s="8"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="G12" s="14" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="13"/>
+      <c r="G12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
-      <c r="K12" s="14" t="s">
+      <c r="H12" s="14"/>
+      <c r="I12" s="13"/>
+      <c r="K12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C13" s="10" t="s">
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="24" t="s">
         <v>23</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>6</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>10</v>
@@ -755,34 +775,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="4"/>
       <c r="G14" s="5"/>
       <c r="I14" s="4"/>
       <c r="K14" s="5"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="4"/>
       <c r="G15" s="5"/>
       <c r="I15" s="4"/>
       <c r="K15" s="5"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="4"/>
       <c r="G16" s="5"/>
       <c r="I16" s="4"/>
       <c r="K16" s="5"/>
@@ -790,7 +813,8 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="4"/>
       <c r="G17" s="5"/>
       <c r="I17" s="4"/>
       <c r="K17" s="5"/>
@@ -798,7 +822,8 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="4"/>
       <c r="G18" s="5"/>
       <c r="I18" s="4"/>
       <c r="K18" s="5"/>
@@ -806,7 +831,8 @@
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="6"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
       <c r="G19" s="6"/>
       <c r="H19" s="7"/>
       <c r="I19" s="8"/>
@@ -815,12 +841,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="C12:E12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor Changes (Table Schema, CRUD)
</commit_message>
<xml_diff>
--- a/ERDiagram-TableSchema/AS2_Excel.xlsx
+++ b/ERDiagram-TableSchema/AS2_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ADA\Subjects\Database Systems\AS2_Git_DBS\ERDiagram-TableSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4EBBEF-D554-4A35-A81C-4A464381EB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C81455C-F35F-449E-82B8-C8206EE812F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>CustomerID</t>
-  </si>
-  <si>
-    <t>FullPrice</t>
   </si>
   <si>
     <t>Orders</t>
@@ -270,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -283,6 +280,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,22 +292,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,7 +578,7 @@
   <dimension ref="A2:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,30 +598,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="18"/>
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="16"/>
+      <c r="J2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="16"/>
       <c r="L2" s="19"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="13"/>
+      <c r="N2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -657,28 +643,26 @@
       <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="L3" s="18"/>
       <c r="N3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="H4" s="4"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="18"/>
       <c r="N4" s="5"/>
       <c r="O4" s="4"/>
     </row>
@@ -686,8 +670,8 @@
       <c r="A5" s="5"/>
       <c r="H5" s="4"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="18"/>
       <c r="N5" s="5"/>
       <c r="O5" s="4"/>
     </row>
@@ -695,8 +679,8 @@
       <c r="A6" s="5"/>
       <c r="H6" s="4"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="18"/>
       <c r="N6" s="5"/>
       <c r="O6" s="4"/>
     </row>
@@ -704,8 +688,8 @@
       <c r="A7" s="5"/>
       <c r="H7" s="4"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="18"/>
       <c r="N7" s="5"/>
       <c r="O7" s="4"/>
     </row>
@@ -713,8 +697,8 @@
       <c r="A8" s="5"/>
       <c r="H8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="18"/>
       <c r="N8" s="5"/>
       <c r="O8" s="4"/>
     </row>
@@ -728,59 +712,58 @@
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="18"/>
       <c r="N9" s="6"/>
       <c r="O9" s="8"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="13"/>
-      <c r="K12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="13"/>
+      <c r="C12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="16"/>
+      <c r="K12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="22" t="s">
+      <c r="D13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="16"/>
       <c r="E14" s="4"/>
       <c r="G14" s="5"/>
       <c r="I14" s="4"/>
@@ -789,10 +772,9 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="16"/>
       <c r="E15" s="4"/>
       <c r="G15" s="5"/>
       <c r="I15" s="4"/>
@@ -801,10 +783,9 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="16"/>
       <c r="E16" s="4"/>
       <c r="G16" s="5"/>
       <c r="I16" s="4"/>
@@ -813,7 +794,6 @@
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
-      <c r="D17" s="16"/>
       <c r="E17" s="4"/>
       <c r="G17" s="5"/>
       <c r="I17" s="4"/>
@@ -822,7 +802,6 @@
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
-      <c r="D18" s="16"/>
       <c r="E18" s="4"/>
       <c r="G18" s="5"/>
       <c r="I18" s="4"/>
@@ -841,12 +820,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="J2:L2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>